<commit_message>
Commit SRC valid register
</commit_message>
<xml_diff>
--- a/docs/Sprint 3 - 2303 To 0504/LogTime.xlsx
+++ b/docs/Sprint 3 - 2303 To 0504/LogTime.xlsx
@@ -464,7 +464,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commit security vs new login HTTP INTERFACE
</commit_message>
<xml_diff>
--- a/docs/Sprint 3 - 2303 To 0504/LogTime.xlsx
+++ b/docs/Sprint 3 - 2303 To 0504/LogTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Column1</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Meeting về data struct và  data flow</t>
   </si>
 </sst>
 </file>
@@ -512,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,6 +811,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>SUM(Table22[24/03/2014])</f>

</xml_diff>